<commit_message>
Custom number formats, floating point support, Time support
</commit_message>
<xml_diff>
--- a/test/files/excel2016.xlsx
+++ b/test/files/excel2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="21105" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="975" yWindow="0" windowWidth="21105" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Basic types" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Some strings</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Baz</t>
   </si>
   <si>
-    <t>Some numbers</t>
-  </si>
-  <si>
     <t>Some empty values</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Some times</t>
   </si>
   <si>
-    <t>Some simple calculations</t>
-  </si>
-  <si>
     <t>Header cell A</t>
   </si>
   <si>
@@ -79,12 +73,27 @@
   </si>
   <si>
     <t>Cell D4</t>
+  </si>
+  <si>
+    <t>Some integer numbers</t>
+  </si>
+  <si>
+    <t>Some decimal numbers</t>
+  </si>
+  <si>
+    <t>Some decimal calculations</t>
+  </si>
+  <si>
+    <t>Some integer calculations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,11 +131,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -407,94 +418,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C2">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="1">
         <v>43881</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <f>B2*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>C2/2</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3">
+        <v>3.75</v>
+      </c>
+      <c r="E3" s="1">
         <v>43882</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.625</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F4" si="0">B3*2</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="0">B3*2</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>C3/2</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="5">
+        <v>4.9989999999999997</v>
+      </c>
+      <c r="E4" s="1">
         <v>43883</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.64236111111111105</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+      <c r="H4">
+        <f>C4/2</f>
+        <v>2.4994999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -507,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -520,35 +560,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial Apple Numbers export compatiblity
</commit_message>
<xml_diff>
--- a/test/files/excel2016.xlsx
+++ b/test/files/excel2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="21105" windowHeight="12840"/>
+    <workbookView xWindow="975" yWindow="0" windowWidth="21105" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic types" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Some strings</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Some integer calculations</t>
+  </si>
+  <si>
+    <t>Row with leading null</t>
+  </si>
+  <si>
+    <t>Row with trailing null</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -545,17 +551,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -591,6 +597,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More compatibility and robustness
</commit_message>
<xml_diff>
--- a/test/files/excel2016.xlsx
+++ b/test/files/excel2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="21105" windowHeight="12840" activeTab="3"/>
+    <workbookView xWindow="1950" yWindow="0" windowWidth="21105" windowHeight="12840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basic types" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Some strings</t>
   </si>
@@ -124,6 +124,22 @@
   </si>
   <si>
     <t>I'm secret</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sharedString is split </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>down the middle</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -133,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +168,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1548,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1647,13 @@
         <v>31</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>